<commit_message>
docs: Update meta tags, add metrics spreadsheet
</commit_message>
<xml_diff>
--- a/site-analysis/PageOverview.xlsx
+++ b/site-analysis/PageOverview.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="105">
   <si>
     <t>Initial implemen- tation</t>
   </si>
@@ -330,6 +330,15 @@
   </si>
   <si>
     <t>Pizzeria</t>
+  </si>
+  <si>
+    <t>Render blocking</t>
+  </si>
+  <si>
+    <t>Optimize delivery</t>
+  </si>
+  <si>
+    <t>Optimize CSS</t>
   </si>
 </sst>
 </file>
@@ -675,10 +684,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I113"/>
+  <dimension ref="A1:I128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="A107" sqref="A107"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -713,495 +722,484 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4">
-        <v>27</v>
+      <c r="A4" s="5" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>5</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B6" t="s">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>8</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B8" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>21</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B14" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B14" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>4</v>
-      </c>
-      <c r="B18">
-        <v>29</v>
+      <c r="A18" s="5" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>5</v>
-      </c>
-      <c r="B19" t="s">
-        <v>6</v>
+        <v>4</v>
+      </c>
+      <c r="B19">
+        <v>71</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>102</v>
+      </c>
       <c r="B20" t="s">
-        <v>7</v>
+        <v>41</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>8</v>
-      </c>
       <c r="B21" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>103</v>
+      </c>
       <c r="B22" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B24" t="s">
-        <v>12</v>
+      <c r="A24" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="B24">
+        <v>76</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>13</v>
-      </c>
-      <c r="B25" t="s">
-        <v>14</v>
+      <c r="A25" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="B25">
+        <v>76</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>20</v>
-      </c>
-      <c r="B26" t="s">
+      <c r="A26" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B26">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B27" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="B28" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="B29" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>21</v>
-      </c>
-      <c r="B27" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B28" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B29" t="s">
-        <v>18</v>
-      </c>
-    </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" s="4"/>
       <c r="B30" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A31" s="2" t="s">
-        <v>23</v>
-      </c>
+      <c r="A31" s="4"/>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>24</v>
-      </c>
-      <c r="B32">
-        <v>51.47</v>
+      <c r="A32" s="2" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="B33">
-        <v>115</v>
+        <v>29</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B34">
-        <v>109</v>
+      <c r="A34" t="s">
+        <v>5</v>
+      </c>
+      <c r="B34" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B35">
-        <v>134</v>
+      <c r="B35" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
+        <v>8</v>
+      </c>
+      <c r="B36" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B37" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B38" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B39" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>13</v>
+      </c>
+      <c r="B40" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>20</v>
+      </c>
+      <c r="B41" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>21</v>
+      </c>
+      <c r="B42" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B43" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B44" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B45" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A46" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>24</v>
+      </c>
+      <c r="B47">
+        <v>51.47</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>25</v>
+      </c>
+      <c r="B48">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B49">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B50">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
         <v>26</v>
       </c>
-      <c r="B36">
+      <c r="B51">
         <v>58.9</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A37" s="2" t="s">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A52" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A38" s="5" t="s">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A53" s="5" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A39" s="5" t="s">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A54" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="B39">
+      <c r="B54">
         <v>16</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A40" s="5" t="s">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A55" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="B40" s="6" t="s">
+      <c r="B55" s="6" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A41" s="5" t="s">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A56" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="B41">
+      <c r="B56">
         <v>454</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A42" s="5" t="s">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A57" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B42">
+      <c r="B57">
         <v>115</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A43" s="5" t="s">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A58" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B43">
+      <c r="B58">
         <v>456</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A44" s="4" t="s">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A59" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B59" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A45" s="4" t="s">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A60" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B60" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A46" s="4" t="s">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A61" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B61" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A47" s="4" t="s">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A62" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B62" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A48" s="4" t="s">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A63" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B63" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A49" s="4" t="s">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A64" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B64" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A50" s="4" t="s">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A65" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B65" t="s">
         <v>54</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A51" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B51" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A52" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B52" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A53" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="B53" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A54" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B54" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A55" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="B55" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A56" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="B56" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A57" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="B57" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A58" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B58" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A59" s="4"/>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A60" s="5" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A61" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="B61">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A62" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="B62">
-        <v>95.6</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A63" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="B63">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A64" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="B64">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A65" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B65">
-        <v>247</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" s="4" t="s">
-        <v>65</v>
+        <v>17</v>
       </c>
       <c r="B66" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B67" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" s="4" t="s">
-        <v>14</v>
+        <v>42</v>
       </c>
       <c r="B68" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69" s="4" t="s">
-        <v>69</v>
+        <v>45</v>
       </c>
       <c r="B69" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" s="4" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="B70" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71" s="4" t="s">
-        <v>17</v>
+        <v>46</v>
       </c>
       <c r="B71" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" s="4" t="s">
-        <v>16</v>
+        <v>47</v>
       </c>
       <c r="B72" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73" s="4" t="s">
-        <v>45</v>
+        <v>18</v>
       </c>
       <c r="B73" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.3">
@@ -1209,7 +1207,7 @@
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75" s="5" t="s">
-        <v>79</v>
+        <v>63</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.3">
@@ -1217,7 +1215,7 @@
         <v>75</v>
       </c>
       <c r="B76">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.3">
@@ -1225,7 +1223,7 @@
         <v>76</v>
       </c>
       <c r="B77">
-        <v>293</v>
+        <v>95.6</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.3">
@@ -1233,7 +1231,7 @@
         <v>77</v>
       </c>
       <c r="B78">
-        <v>168</v>
+        <v>245</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.3">
@@ -1241,7 +1239,7 @@
         <v>64</v>
       </c>
       <c r="B79">
-        <v>95</v>
+        <v>197</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.3">
@@ -1249,15 +1247,15 @@
         <v>44</v>
       </c>
       <c r="B80">
-        <v>169</v>
+        <v>247</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81" s="4" t="s">
-        <v>80</v>
+        <v>65</v>
       </c>
       <c r="B81" t="s">
-        <v>81</v>
+        <v>66</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.3">
@@ -1265,7 +1263,7 @@
         <v>15</v>
       </c>
       <c r="B82" t="s">
-        <v>82</v>
+        <v>67</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.3">
@@ -1273,15 +1271,15 @@
         <v>14</v>
       </c>
       <c r="B83" t="s">
-        <v>83</v>
+        <v>68</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A84" s="4" t="s">
-        <v>41</v>
+        <v>69</v>
       </c>
       <c r="B84" t="s">
-        <v>52</v>
+        <v>70</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.3">
@@ -1289,7 +1287,7 @@
         <v>41</v>
       </c>
       <c r="B85" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.3">
@@ -1297,7 +1295,7 @@
         <v>17</v>
       </c>
       <c r="B86" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.3">
@@ -1305,7 +1303,7 @@
         <v>16</v>
       </c>
       <c r="B87" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.3">
@@ -1313,87 +1311,87 @@
         <v>45</v>
       </c>
       <c r="B88" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A89" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="B89" t="s">
-        <v>89</v>
-      </c>
+      <c r="A89" s="4"/>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A90" s="4"/>
+      <c r="A90" s="5" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A91" s="5" t="s">
-        <v>90</v>
+        <v>75</v>
+      </c>
+      <c r="B91">
+        <v>9</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A92" s="5" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B92">
-        <v>9</v>
+        <v>293</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A93" s="5" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B93">
-        <v>217</v>
+        <v>168</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A94" s="5" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="B94">
-        <v>197</v>
+        <v>95</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A95" s="5" t="s">
-        <v>64</v>
+        <v>44</v>
       </c>
       <c r="B95">
-        <v>87</v>
+        <v>169</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A96" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B96">
-        <v>199</v>
+      <c r="A96" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B96" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A97" s="4" t="s">
-        <v>91</v>
+        <v>15</v>
       </c>
       <c r="B97" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A98" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B98" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A99" s="4" t="s">
-        <v>14</v>
+        <v>41</v>
       </c>
       <c r="B99" t="s">
-        <v>95</v>
+        <v>52</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.3">
@@ -1401,23 +1399,23 @@
         <v>41</v>
       </c>
       <c r="B100" t="s">
-        <v>52</v>
+        <v>84</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A101" s="4" t="s">
-        <v>41</v>
+        <v>17</v>
       </c>
       <c r="B101" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A102" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B102" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.3">
@@ -1425,78 +1423,190 @@
         <v>45</v>
       </c>
       <c r="B103" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A104" s="4" t="s">
-        <v>16</v>
+        <v>85</v>
       </c>
       <c r="B104" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A105" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="B105" t="s">
-        <v>100</v>
-      </c>
+      <c r="A105" s="4"/>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A106" s="4"/>
+      <c r="A106" s="5" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A107" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B107">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A108" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B108">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A109" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B109">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A110" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B110">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A111" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B111">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A112" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="B112" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A113" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B113" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A114" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B114" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A115" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B115" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A116" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B116" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A117" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B117" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A118" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B118" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A119" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B119" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A120" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B120" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A121" s="4"/>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A122" s="5" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A108" t="s">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A123" t="s">
         <v>27</v>
       </c>
-      <c r="B108" t="s">
+      <c r="B123" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A109" t="s">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A124" t="s">
         <v>18</v>
       </c>
-      <c r="B109" t="s">
+      <c r="B124" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A110" t="s">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A125" t="s">
         <v>15</v>
       </c>
-      <c r="B110" t="s">
+      <c r="B125" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A111" t="s">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A126" t="s">
         <v>30</v>
       </c>
-      <c r="B111" t="s">
+      <c r="B126" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A112" t="s">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A127" t="s">
         <v>28</v>
       </c>
-      <c r="B112" t="s">
+      <c r="B127" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A113" t="s">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A128" t="s">
         <v>29</v>
       </c>
-      <c r="B113" t="s">
+      <c r="B128" t="s">
         <v>37</v>
       </c>
     </row>

</xml_diff>